<commit_message>
deal with empty missingConditionDate rows (dzhw/metadatamanagement#1608)
</commit_message>
<xml_diff>
--- a/inst/extdata/excel/vimport_ds1.xlsx
+++ b/inst/extdata/excel/vimport_ds1.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">generationDetails.ruleExpressionLanguage</t>
   </si>
   <si>
-    <t xml:space="preserve">panelIdentifier</t>
+    <t xml:space="preserve">repeatedMeasurementIdentifier</t>
   </si>
   <si>
     <t xml:space="preserve">relatedVariables</t>
@@ -369,8 +369,8 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -530,8 +530,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -544,10 +544,10 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="C2:C4 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="73.01"/>

</xml_diff>